<commit_message>
v1.3.0 save for fixed excel file
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/20200706.xlsx
+++ b/ai/assets/textbook/pinyin/20200706.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15F9F10-83B6-4A95-B47F-1123B71969D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B49F00D-F785-41EB-93C2-565EF14A0B01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1170" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22170" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$B$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$B$447</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="441">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -323,18 +323,6 @@
     <t>&lt;msg&gt;&lt;at&gt;你的名字;D53171028365&lt;/at&gt; 喜欢舔&lt;lv&gt;15&lt;/lv&gt;&lt;/msg&gt;</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;0-10-22-30&lt;/dt&gt;&lt;at&gt;***ag81@点cc&lt;/at&gt; &lt;at&gt;AG官网&lt;/at&gt; &lt;at&gt;小耗子&lt;/at&gt; &lt;a</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-10-10-26&lt;/dt&gt;杀老板全家，老板全家的女的全部被奸杀&lt;isAncho</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-10-12-28&lt;/dt&gt;你的面子算个鸡掰&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfo</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-10-5-13&lt;/dt&gt;死妈&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-10-5-21&lt;/dt&gt;水很多，滑滑的就进去了&lt;isAnchorPlatformMsg&gt;0&lt;/isAnch</t>
   </si>
   <si>
@@ -365,9 +353,6 @@
     <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-11-12-29&lt;/dt&gt;后台的人员，生孩子没屁眼的东西&lt;isAnchorPlatform</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-11-5-28&lt;/dt&gt;&lt;at&gt;花花看看b我给你刷礼物&lt;/at&gt;&lt;isAnchorPlatformMsg&gt;0&lt;</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-11-9-26&lt;/dt&gt;你老妈啊，&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/ms</t>
   </si>
   <si>
@@ -377,9 +362,6 @@
     <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-2-5-22&lt;/dt&gt;全家不得好死，乱来，你坑钱去买棺材吗&lt;isAnchorP</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-2-5-23&lt;/dt&gt;&lt;at&gt;一定要有花恭祝AG全体人员被车撞死&lt;/at&gt;&lt;isAncho</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;0&lt;/yplv&gt;&lt;dt&gt;1-2-5-27&lt;/dt&gt;畜牲&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
   </si>
   <si>
@@ -455,9 +437,6 @@
     <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-19&lt;/dt&gt;花花，我想干你屁眼&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlat</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-21&lt;/dt&gt;&lt;at&gt;又菲洗澡让你玩鸟&lt;/at&gt;&lt;isAnchorPlatformMsg&gt;0&lt;/isAnch</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-21&lt;/dt&gt;杀尼吗&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
   </si>
   <si>
@@ -467,9 +446,6 @@
     <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-25&lt;/dt&gt;老板全家都死光了不杀点棺材钱怎么行&lt;isAnchorPla</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-26&lt;/dt&gt;&lt;at&gt;花花我很会舔的，相信我，你会很舒服&lt;/at&gt;&lt;is</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;2&lt;/yplv&gt;&lt;dt&gt;1-10-5-9&lt;/dt&gt;老板和所有幕后的人，祝你们全家早点死光&lt;isAnch</t>
   </si>
   <si>
@@ -590,136 +566,19 @@
     <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-0-7-29&lt;/dt&gt;老板死了跑什么&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-14&lt;/dt&gt;我也想干主播&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-22&lt;/dt&gt;老板家人死光光了急需用钱就这样坑骗我们玩家</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-22&lt;/dt&gt;花花多少钱包夜&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMs</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-26&lt;/dt&gt;老板你不得好死&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMs</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-26&lt;/dt&gt;走人，等老板吗死了再来开金庆祝&lt;isAnchorPlatformM</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-5-27&lt;/dt&gt;庄家死绝种，最好，骗人钱&lt;isAnchorPlatformMsg&gt;0&lt;/isA</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-7-27&lt;/dt&gt;老板你全家不得好死&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlat</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-10-8-24&lt;/dt&gt;我昨晚睡觉后台的女儿，才给后台杀了&lt;isAnchorPla</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-1-5-27&lt;/dt&gt;安娜 你下面是不是黑的&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorP</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-2-5-10&lt;/dt&gt;组队去干花花，有人么&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPl</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-2-5-14&lt;/dt&gt;死妈庄家&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-10-5-25&lt;/dt&gt;畜牲&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-0-9-29&lt;/dt&gt;老板死了全家&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-10-5-11&lt;/dt&gt;快射金了&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
   </si>
   <si>
     <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-10-5-14&lt;/dt&gt;畜牲&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-10-5-26&lt;/dt&gt;昨天我才去看他回来，老板全家是真的得艾滋和</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-10-8-23&lt;/dt&gt;后台父母双亡&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;</t>
-  </si>
-  <si>
     <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-11-14-29&lt;/dt&gt;嘛嘛批&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
   </si>
   <si>
     <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-11-7-29&lt;/dt&gt;贱&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-2-5-19&lt;/dt&gt;把主播塞满&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;dt&gt;1-2-5-28&lt;/dt&gt;全家暴毙&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-10-5-23&lt;/dt&gt;这游戏的老板不得好死&lt;isAnchorPlatformMsg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-11&lt;/dt&gt;暖暖奶小B大&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/m</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-19&lt;/dt&gt;野鸡注册送88&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-22&lt;/dt&gt;我特码要干你祖宗&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfor</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-23&lt;/dt&gt;主播不看片，主播就喜欢自己玩自己&lt;isAnchorPlatfo</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-24&lt;/dt&gt;去国际网络赌博刑侦大队搞&lt;isAnchorPlatformMsg&gt;0&lt;/isA</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-10-5-25&lt;/dt&gt;老板全家不得好死&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfor</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;dt&gt;1-11-11-27&lt;/dt&gt;你大爷的&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-1-5-28&lt;/dt&gt;畜牲 这样杀持续几天了&lt;isAnchorPlatformMsg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-1-6-27&lt;/dt&gt;真特么畜牲 &lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlat</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-1-6-28&lt;/dt&gt;畜牲老板&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatform</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;7&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-1-7-28&lt;/dt&gt;谁玩谁是这个贱比&lt;isAnchorPlatformMsg&gt;0&lt;/isAn</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;0-10-11-29&lt;/dt&gt;超老板全家&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/m</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-10-5-28&lt;/dt&gt;我也想干她&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/ms</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-10-9-28&lt;/dt&gt;老板得冠性病毒了，要买棺材&lt;isAnchorPlatformMsg&gt;0&lt;/</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-11-5-20&lt;/dt&gt;老板全家癌症晚期&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfor</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-11-5-22&lt;/dt&gt;老板全家癌症&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-11-5-24&lt;/dt&gt;老板全家癌症晚期&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfor</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-11-5-25&lt;/dt&gt;猪播B贱！&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-11-7-28&lt;/dt&gt;这个主播就是梅比&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfor</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-1-5-24&lt;/dt&gt;畜牲&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;dt&gt;1-2-5-9&lt;/dt&gt;都把基吧割了就赢了&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatfo</t>
-  </si>
-  <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;8&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-10-5-20&lt;/dt&gt;&lt;at&gt;稳住你嫁我15116638343我看看&lt;/at&gt;&lt;isAnch</t>
   </si>
   <si>
     <t>&lt;msg&gt;MMP不玩了，手工&lt;lv&gt;11&lt;/lv&gt;&lt;/msg&gt;</t>
@@ -1385,6 +1244,166 @@
   </si>
   <si>
     <t>&lt;msg&gt;两个字，畜牲&lt;lv&gt;12&lt;/lv&gt;&lt;/msg&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀老板全家，老板全家的女的全部被奸杀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的面子算个鸡掰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>死妈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳住你嫁我15116638343我看看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>都把基吧割了就赢了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>畜牲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个主播就是梅比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猪播B贱！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板全家癌症晚期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板全家癌症</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板得冠性病毒了，要买棺材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我也想干她</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超老板全家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谁玩谁是这个贱比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>畜牲老板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真特么畜牲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>畜牲 这样杀持续几天了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你大爷的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板全家不得好死</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去国际网络赌博刑侦大队搞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主播不看片，主播就喜欢自己玩自己</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我特码要干你祖宗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>野鸡注册送88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暖暖奶小B大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这游戏的老板不得好死</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全家暴毙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把主播塞满</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台父母双亡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昨天我才去看他回来，老板全家是真的得艾滋和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板死了全家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;msg&gt;&lt;yplv&gt;5&lt;/yplv&gt;&lt;dt&gt;1-2-5-14&lt;/dt&gt;死妈庄家&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMsg&gt;&lt;/msg&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组队去干花花，有人么</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安娜 你下面是不是黑的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我昨晚睡觉后台的女儿，才给后台杀了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板你全家不得好死</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>庄家死绝种，最好，骗人钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>走人，等老板吗死了再来开金庆祝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老板你不得好死</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花花多少钱包夜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我也想干主播</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1723,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B452"/>
+  <dimension ref="A1:B447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="A252" sqref="A252"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="A277" sqref="A277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2457,7 +2476,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>440</v>
+        <v>393</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2505,7 +2524,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>401</v>
       </c>
       <c r="B97">
         <v>4</v>
@@ -2513,7 +2532,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>402</v>
       </c>
       <c r="B98">
         <v>4</v>
@@ -2521,7 +2540,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>99</v>
+        <v>403</v>
       </c>
       <c r="B99">
         <v>4</v>
@@ -2529,7 +2548,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B100">
         <v>4</v>
@@ -2537,7 +2556,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B101">
         <v>4</v>
@@ -2545,7 +2564,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B102">
         <v>4</v>
@@ -2553,7 +2572,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B103">
         <v>4</v>
@@ -2561,7 +2580,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>4</v>
@@ -2569,7 +2588,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B105">
         <v>4</v>
@@ -2577,7 +2596,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B106">
         <v>4</v>
@@ -2585,7 +2604,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B107">
         <v>4</v>
@@ -2593,7 +2612,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B108">
         <v>4</v>
@@ -2601,7 +2620,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B109">
         <v>4</v>
@@ -2609,7 +2628,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B110">
         <v>4</v>
@@ -2617,7 +2636,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B111">
         <v>4</v>
@@ -2625,7 +2644,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B112">
         <v>4</v>
@@ -2633,7 +2652,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B113">
         <v>4</v>
@@ -2641,7 +2660,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B114">
         <v>4</v>
@@ -2649,7 +2668,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -2657,7 +2676,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B116">
         <v>4</v>
@@ -2665,7 +2684,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B117">
         <v>4</v>
@@ -2673,7 +2692,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B118">
         <v>4</v>
@@ -2681,7 +2700,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B119">
         <v>4</v>
@@ -2689,7 +2708,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B120">
         <v>4</v>
@@ -2697,7 +2716,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B121">
         <v>4</v>
@@ -2705,7 +2724,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B122">
         <v>4</v>
@@ -2713,7 +2732,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B123">
         <v>4</v>
@@ -2721,7 +2740,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B124">
         <v>4</v>
@@ -2729,7 +2748,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B125">
         <v>4</v>
@@ -2737,7 +2756,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B126">
         <v>4</v>
@@ -2745,7 +2764,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B127">
         <v>4</v>
@@ -2753,7 +2772,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B128">
         <v>4</v>
@@ -2761,7 +2780,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B129">
         <v>4</v>
@@ -2769,7 +2788,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B130">
         <v>4</v>
@@ -2777,7 +2796,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B131">
         <v>4</v>
@@ -2785,7 +2804,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B132">
         <v>4</v>
@@ -2793,7 +2812,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B133">
         <v>4</v>
@@ -2801,7 +2820,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B134">
         <v>4</v>
@@ -2809,7 +2828,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B135">
         <v>4</v>
@@ -2817,7 +2836,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B136">
         <v>4</v>
@@ -2825,7 +2844,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B137">
         <v>4</v>
@@ -2833,7 +2852,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B138">
         <v>4</v>
@@ -2841,7 +2860,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -2849,7 +2868,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B140">
         <v>4</v>
@@ -2857,7 +2876,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B141">
         <v>4</v>
@@ -2865,7 +2884,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B142">
         <v>4</v>
@@ -2873,7 +2892,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B143">
         <v>4</v>
@@ -2881,7 +2900,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B144">
         <v>4</v>
@@ -2889,7 +2908,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B145">
         <v>4</v>
@@ -2897,7 +2916,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B146">
         <v>4</v>
@@ -2905,7 +2924,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B147">
         <v>4</v>
@@ -2913,7 +2932,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B148">
         <v>4</v>
@@ -2921,7 +2940,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B149">
         <v>4</v>
@@ -2929,7 +2948,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B150">
         <v>4</v>
@@ -2937,7 +2956,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B151">
         <v>4</v>
@@ -2945,7 +2964,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B152">
         <v>4</v>
@@ -2953,7 +2972,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B153">
         <v>4</v>
@@ -2961,7 +2980,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B154">
         <v>4</v>
@@ -2969,7 +2988,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B155">
         <v>4</v>
@@ -2977,7 +2996,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B156">
         <v>4</v>
@@ -2985,7 +3004,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B157">
         <v>4</v>
@@ -2993,7 +3012,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B158">
         <v>4</v>
@@ -3001,7 +3020,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B159">
         <v>4</v>
@@ -3009,7 +3028,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B160">
         <v>4</v>
@@ -3017,7 +3036,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B161">
         <v>4</v>
@@ -3025,7 +3044,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B162">
         <v>4</v>
@@ -3033,7 +3052,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -3041,7 +3060,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B164">
         <v>4</v>
@@ -3049,7 +3068,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B165">
         <v>4</v>
@@ -3057,7 +3076,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B166">
         <v>4</v>
@@ -3065,7 +3084,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B167">
         <v>4</v>
@@ -3073,7 +3092,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B168">
         <v>4</v>
@@ -3081,7 +3100,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B169">
         <v>4</v>
@@ -3089,7 +3108,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B170">
         <v>4</v>
@@ -3097,7 +3116,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B171">
         <v>4</v>
@@ -3105,7 +3124,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B172">
         <v>4</v>
@@ -3113,7 +3132,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B173">
         <v>4</v>
@@ -3121,7 +3140,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B174">
         <v>4</v>
@@ -3129,7 +3148,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B175">
         <v>4</v>
@@ -3137,7 +3156,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B176">
         <v>4</v>
@@ -3145,7 +3164,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B177">
         <v>4</v>
@@ -3153,7 +3172,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B178">
         <v>4</v>
@@ -3161,7 +3180,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B179">
         <v>4</v>
@@ -3169,7 +3188,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B180">
         <v>4</v>
@@ -3177,7 +3196,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>181</v>
+        <v>440</v>
       </c>
       <c r="B181">
         <v>4</v>
@@ -3185,7 +3204,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B182">
         <v>4</v>
@@ -3193,7 +3212,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>183</v>
+        <v>439</v>
       </c>
       <c r="B183">
         <v>4</v>
@@ -3201,7 +3220,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>184</v>
+        <v>438</v>
       </c>
       <c r="B184">
         <v>4</v>
@@ -3209,7 +3228,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>185</v>
+        <v>437</v>
       </c>
       <c r="B185">
         <v>4</v>
@@ -3217,7 +3236,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>186</v>
+        <v>436</v>
       </c>
       <c r="B186">
         <v>4</v>
@@ -3225,7 +3244,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>187</v>
+        <v>435</v>
       </c>
       <c r="B187">
         <v>4</v>
@@ -3233,7 +3252,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>188</v>
+        <v>434</v>
       </c>
       <c r="B188">
         <v>4</v>
@@ -3241,7 +3260,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>189</v>
+        <v>433</v>
       </c>
       <c r="B189">
         <v>4</v>
@@ -3249,7 +3268,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>190</v>
+        <v>432</v>
       </c>
       <c r="B190">
         <v>4</v>
@@ -3257,7 +3276,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>191</v>
+        <v>431</v>
       </c>
       <c r="B191">
         <v>4</v>
@@ -3265,7 +3284,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>192</v>
+        <v>406</v>
       </c>
       <c r="B192">
         <v>4</v>
@@ -3273,7 +3292,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>193</v>
+        <v>430</v>
       </c>
       <c r="B193">
         <v>4</v>
@@ -3281,7 +3300,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B194">
         <v>4</v>
@@ -3289,7 +3308,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B195">
         <v>4</v>
@@ -3297,7 +3316,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>196</v>
+        <v>429</v>
       </c>
       <c r="B196">
         <v>4</v>
@@ -3305,7 +3324,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>197</v>
+        <v>428</v>
       </c>
       <c r="B197">
         <v>4</v>
@@ -3313,7 +3332,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B198">
         <v>4</v>
@@ -3321,7 +3340,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B199">
         <v>4</v>
@@ -3329,7 +3348,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>200</v>
+        <v>427</v>
       </c>
       <c r="B200">
         <v>4</v>
@@ -3337,7 +3356,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>201</v>
+        <v>426</v>
       </c>
       <c r="B201">
         <v>4</v>
@@ -3345,7 +3364,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>202</v>
+        <v>425</v>
       </c>
       <c r="B202">
         <v>4</v>
@@ -3353,7 +3372,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>203</v>
+        <v>424</v>
       </c>
       <c r="B203">
         <v>4</v>
@@ -3361,7 +3380,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>204</v>
+        <v>423</v>
       </c>
       <c r="B204">
         <v>4</v>
@@ -3369,7 +3388,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>205</v>
+        <v>422</v>
       </c>
       <c r="B205">
         <v>4</v>
@@ -3377,7 +3396,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>206</v>
+        <v>421</v>
       </c>
       <c r="B206">
         <v>4</v>
@@ -3385,7 +3404,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>207</v>
+        <v>420</v>
       </c>
       <c r="B207">
         <v>4</v>
@@ -3393,7 +3412,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>208</v>
+        <v>419</v>
       </c>
       <c r="B208">
         <v>4</v>
@@ -3401,7 +3420,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>209</v>
+        <v>418</v>
       </c>
       <c r="B209">
         <v>4</v>
@@ -3409,7 +3428,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>210</v>
+        <v>417</v>
       </c>
       <c r="B210">
         <v>4</v>
@@ -3417,7 +3436,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>211</v>
+        <v>416</v>
       </c>
       <c r="B211">
         <v>4</v>
@@ -3425,7 +3444,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>212</v>
+        <v>415</v>
       </c>
       <c r="B212">
         <v>4</v>
@@ -3433,7 +3452,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>213</v>
+        <v>414</v>
       </c>
       <c r="B213">
         <v>4</v>
@@ -3441,7 +3460,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>214</v>
+        <v>413</v>
       </c>
       <c r="B214">
         <v>4</v>
@@ -3449,7 +3468,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>215</v>
+        <v>412</v>
       </c>
       <c r="B215">
         <v>4</v>
@@ -3457,7 +3476,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>216</v>
+        <v>411</v>
       </c>
       <c r="B216">
         <v>4</v>
@@ -3465,7 +3484,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>217</v>
+        <v>409</v>
       </c>
       <c r="B217">
         <v>4</v>
@@ -3473,7 +3492,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>218</v>
+        <v>410</v>
       </c>
       <c r="B218">
         <v>4</v>
@@ -3481,7 +3500,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>219</v>
+        <v>409</v>
       </c>
       <c r="B219">
         <v>4</v>
@@ -3489,7 +3508,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>220</v>
+        <v>408</v>
       </c>
       <c r="B220">
         <v>4</v>
@@ -3497,7 +3516,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>221</v>
+        <v>407</v>
       </c>
       <c r="B221">
         <v>4</v>
@@ -3505,7 +3524,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>222</v>
+        <v>406</v>
       </c>
       <c r="B222">
         <v>4</v>
@@ -3513,7 +3532,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>223</v>
+        <v>405</v>
       </c>
       <c r="B223">
         <v>4</v>
@@ -3521,15 +3540,15 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>224</v>
+        <v>404</v>
       </c>
       <c r="B224">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="B225">
         <v>4</v>
@@ -3537,7 +3556,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B226">
         <v>4</v>
@@ -3545,7 +3564,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="B227">
         <v>4</v>
@@ -3553,7 +3572,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="B228">
         <v>4</v>
@@ -3561,15 +3580,15 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="B229">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="B230">
         <v>4</v>
@@ -3577,7 +3596,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="B231">
         <v>4</v>
@@ -3585,7 +3604,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="B232">
         <v>4</v>
@@ -3593,7 +3612,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="B233">
         <v>4</v>
@@ -3601,7 +3620,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="B234">
         <v>4</v>
@@ -3609,7 +3628,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="B235">
         <v>4</v>
@@ -3617,7 +3636,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="B236">
         <v>4</v>
@@ -3625,7 +3644,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B237">
         <v>4</v>
@@ -3633,7 +3652,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>238</v>
+        <v>400</v>
       </c>
       <c r="B238">
         <v>4</v>
@@ -3641,7 +3660,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="B239">
         <v>4</v>
@@ -3649,7 +3668,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="B240">
         <v>4</v>
@@ -3657,7 +3676,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="B241">
         <v>4</v>
@@ -3665,7 +3684,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>242</v>
+        <v>399</v>
       </c>
       <c r="B242">
         <v>4</v>
@@ -3673,7 +3692,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>447</v>
+        <v>199</v>
       </c>
       <c r="B243">
         <v>4</v>
@@ -3681,7 +3700,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="B244">
         <v>4</v>
@@ -3689,7 +3708,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="B245">
         <v>4</v>
@@ -3697,7 +3716,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="B246">
         <v>4</v>
@@ -3705,55 +3724,55 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>446</v>
+        <v>203</v>
       </c>
       <c r="B247">
         <v>4</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
-        <v>246</v>
+      <c r="A248" t="s">
+        <v>204</v>
       </c>
       <c r="B248">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
-        <v>247</v>
+      <c r="A249" t="s">
+        <v>205</v>
       </c>
       <c r="B249">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>248</v>
+      <c r="A250" t="s">
+        <v>398</v>
       </c>
       <c r="B250">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
-        <v>249</v>
+      <c r="A251" t="s">
+        <v>206</v>
       </c>
       <c r="B251">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
-        <v>250</v>
+      <c r="A252" t="s">
+        <v>207</v>
       </c>
       <c r="B252">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>251</v>
+        <v>208</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -3761,15 +3780,15 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>252</v>
+        <v>209</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>445</v>
+        <v>210</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -3777,7 +3796,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>253</v>
+        <v>211</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -3785,7 +3804,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -3793,7 +3812,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -3801,15 +3820,15 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
       <c r="B259">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -3817,7 +3836,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -3825,7 +3844,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -3833,7 +3852,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -3841,7 +3860,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>261</v>
+        <v>219</v>
       </c>
       <c r="B264">
         <v>1</v>
@@ -3849,7 +3868,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -3857,7 +3876,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -3865,7 +3884,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>264</v>
+        <v>397</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -3873,7 +3892,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>265</v>
+        <v>394</v>
       </c>
       <c r="B268">
         <v>1</v>
@@ -3881,7 +3900,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>266</v>
+        <v>222</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -3889,7 +3908,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -3897,7 +3916,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -3905,7 +3924,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>444</v>
+        <v>395</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -3913,7 +3932,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>441</v>
+        <v>225</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -3921,7 +3940,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -3929,7 +3948,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="B275">
         <v>1</v>
@@ -3937,7 +3956,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>271</v>
+        <v>396</v>
       </c>
       <c r="B276">
         <v>1</v>
@@ -3945,15 +3964,15 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>442</v>
+        <v>228</v>
       </c>
       <c r="B277">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="B278">
         <v>1</v>
@@ -3961,7 +3980,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="B279">
         <v>1</v>
@@ -3969,7 +3988,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B280">
         <v>1</v>
@@ -3977,7 +3996,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>443</v>
+        <v>232</v>
       </c>
       <c r="B281">
         <v>1</v>
@@ -3985,7 +4004,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>275</v>
+        <v>233</v>
       </c>
       <c r="B282">
         <v>1</v>
@@ -3993,7 +4012,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
       <c r="B283">
         <v>1</v>
@@ -4001,7 +4020,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>277</v>
+        <v>235</v>
       </c>
       <c r="B284">
         <v>1</v>
@@ -4009,7 +4028,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -4017,7 +4036,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -4025,7 +4044,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -4033,7 +4052,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="B288">
         <v>1</v>
@@ -4041,7 +4060,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -4049,7 +4068,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>282</v>
+        <v>240</v>
       </c>
       <c r="B290">
         <v>1</v>
@@ -4057,7 +4076,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>283</v>
+        <v>241</v>
       </c>
       <c r="B291">
         <v>1</v>
@@ -4065,7 +4084,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>284</v>
+        <v>242</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -4073,7 +4092,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>285</v>
+        <v>243</v>
       </c>
       <c r="B293">
         <v>1</v>
@@ -4081,7 +4100,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>286</v>
+        <v>244</v>
       </c>
       <c r="B294">
         <v>1</v>
@@ -4089,15 +4108,15 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="B295">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>288</v>
+        <v>246</v>
       </c>
       <c r="B296">
         <v>1</v>
@@ -4105,7 +4124,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
       <c r="B297">
         <v>1</v>
@@ -4113,7 +4132,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="B298">
         <v>1</v>
@@ -4121,23 +4140,23 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>291</v>
+        <v>249</v>
       </c>
       <c r="B299">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
       <c r="B300">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -4145,7 +4164,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="B302">
         <v>1</v>
@@ -4153,7 +4172,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="B303">
         <v>1</v>
@@ -4161,15 +4180,15 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="B304">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B305">
         <v>1</v>
@@ -4177,7 +4196,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="B306">
         <v>1</v>
@@ -4185,7 +4204,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="B307">
         <v>1</v>
@@ -4193,7 +4212,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>299</v>
+        <v>257</v>
       </c>
       <c r="B308">
         <v>1</v>
@@ -4201,7 +4220,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="B309">
         <v>1</v>
@@ -4209,7 +4228,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>301</v>
+        <v>259</v>
       </c>
       <c r="B310">
         <v>1</v>
@@ -4217,7 +4236,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>302</v>
+        <v>260</v>
       </c>
       <c r="B311">
         <v>1</v>
@@ -4225,7 +4244,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>303</v>
+        <v>261</v>
       </c>
       <c r="B312">
         <v>1</v>
@@ -4233,7 +4252,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>304</v>
+        <v>262</v>
       </c>
       <c r="B313">
         <v>1</v>
@@ -4241,7 +4260,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="B314">
         <v>1</v>
@@ -4249,7 +4268,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
       <c r="B315">
         <v>1</v>
@@ -4257,7 +4276,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="B316">
         <v>1</v>
@@ -4265,7 +4284,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>308</v>
+        <v>266</v>
       </c>
       <c r="B317">
         <v>1</v>
@@ -4273,7 +4292,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>309</v>
+        <v>267</v>
       </c>
       <c r="B318">
         <v>1</v>
@@ -4281,7 +4300,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>310</v>
+        <v>268</v>
       </c>
       <c r="B319">
         <v>1</v>
@@ -4289,7 +4308,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
       <c r="B320">
         <v>1</v>
@@ -4297,7 +4316,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>312</v>
+        <v>270</v>
       </c>
       <c r="B321">
         <v>1</v>
@@ -4305,7 +4324,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>313</v>
+        <v>271</v>
       </c>
       <c r="B322">
         <v>1</v>
@@ -4313,15 +4332,15 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>314</v>
+        <v>272</v>
       </c>
       <c r="B323">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
       <c r="B324">
         <v>1</v>
@@ -4329,7 +4348,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
       <c r="B325">
         <v>1</v>
@@ -4337,7 +4356,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="B326">
         <v>1</v>
@@ -4345,7 +4364,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="B327">
         <v>1</v>
@@ -4353,15 +4372,15 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="B328">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="B329">
         <v>1</v>
@@ -4369,7 +4388,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
       <c r="B330">
         <v>1</v>
@@ -4377,7 +4396,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
       <c r="B331">
         <v>1</v>
@@ -4385,7 +4404,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="B332">
         <v>1</v>
@@ -4393,7 +4412,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="B333">
         <v>1</v>
@@ -4401,7 +4420,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="B334">
         <v>1</v>
@@ -4409,7 +4428,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
       <c r="B335">
         <v>1</v>
@@ -4417,7 +4436,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>327</v>
+        <v>285</v>
       </c>
       <c r="B336">
         <v>1</v>
@@ -4425,7 +4444,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>328</v>
+        <v>286</v>
       </c>
       <c r="B337">
         <v>1</v>
@@ -4433,7 +4452,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>329</v>
+        <v>287</v>
       </c>
       <c r="B338">
         <v>1</v>
@@ -4441,7 +4460,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="B339">
         <v>1</v>
@@ -4449,7 +4468,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>331</v>
+        <v>289</v>
       </c>
       <c r="B340">
         <v>1</v>
@@ -4457,7 +4476,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="B341">
         <v>1</v>
@@ -4465,7 +4484,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>333</v>
+        <v>2</v>
       </c>
       <c r="B342">
         <v>1</v>
@@ -4473,7 +4492,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="B343">
         <v>1</v>
@@ -4481,7 +4500,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="B344">
         <v>1</v>
@@ -4489,7 +4508,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B345">
         <v>1</v>
@@ -4497,7 +4516,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B346">
         <v>1</v>
@@ -4505,7 +4524,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>2</v>
+        <v>295</v>
       </c>
       <c r="B347">
         <v>1</v>
@@ -4513,15 +4532,15 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
       <c r="B348">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="B349">
         <v>1</v>
@@ -4529,7 +4548,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="B350">
         <v>1</v>
@@ -4537,7 +4556,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="B351">
         <v>1</v>
@@ -4545,7 +4564,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="B352">
         <v>1</v>
@@ -4553,15 +4572,15 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="B353">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="B354">
         <v>1</v>
@@ -4569,7 +4588,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="B355">
         <v>1</v>
@@ -4577,7 +4596,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="B356">
         <v>1</v>
@@ -4585,7 +4604,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="B357">
         <v>1</v>
@@ -4593,7 +4612,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="B358">
         <v>1</v>
@@ -4601,7 +4620,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="B359">
         <v>1</v>
@@ -4609,7 +4628,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="B360">
         <v>1</v>
@@ -4617,7 +4636,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="B361">
         <v>1</v>
@@ -4625,7 +4644,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="B362">
         <v>1</v>
@@ -4633,7 +4652,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="B363">
         <v>1</v>
@@ -4641,7 +4660,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
       <c r="B364">
         <v>1</v>
@@ -4649,7 +4668,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="B365">
         <v>1</v>
@@ -4657,7 +4676,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="B366">
         <v>1</v>
@@ -4665,7 +4684,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="B367">
         <v>1</v>
@@ -4673,7 +4692,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="B368">
         <v>1</v>
@@ -4681,7 +4700,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
       <c r="B369">
         <v>1</v>
@@ -4689,7 +4708,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="B370">
         <v>1</v>
@@ -4697,7 +4716,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="B371">
         <v>1</v>
@@ -4705,7 +4724,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
       <c r="B372">
         <v>1</v>
@@ -4713,7 +4732,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="B373">
         <v>1</v>
@@ -4721,47 +4740,47 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="B374">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="B375">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="B376">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
       <c r="B377">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="B378">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="B379">
         <v>4</v>
@@ -4769,47 +4788,47 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="B380">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>371</v>
+        <v>329</v>
       </c>
       <c r="B381">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
       <c r="B382">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
       <c r="B383">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="B384">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="B385">
         <v>1</v>
@@ -4817,7 +4836,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="B386">
         <v>1</v>
@@ -4825,7 +4844,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="B387">
         <v>1</v>
@@ -4833,7 +4852,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="B388">
         <v>1</v>
@@ -4841,7 +4860,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>378</v>
+        <v>336</v>
       </c>
       <c r="B389">
         <v>1</v>
@@ -4849,7 +4868,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>379</v>
+        <v>337</v>
       </c>
       <c r="B390">
         <v>1</v>
@@ -4857,7 +4876,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="B391">
         <v>1</v>
@@ -4865,7 +4884,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
       <c r="B392">
         <v>1</v>
@@ -4873,7 +4892,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>382</v>
+        <v>340</v>
       </c>
       <c r="B393">
         <v>1</v>
@@ -4881,7 +4900,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="B394">
         <v>1</v>
@@ -4889,7 +4908,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>384</v>
+        <v>342</v>
       </c>
       <c r="B395">
         <v>1</v>
@@ -4897,7 +4916,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="B396">
         <v>1</v>
@@ -4905,7 +4924,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="B397">
         <v>1</v>
@@ -4913,7 +4932,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>387</v>
+        <v>345</v>
       </c>
       <c r="B398">
         <v>1</v>
@@ -4921,7 +4940,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>388</v>
+        <v>346</v>
       </c>
       <c r="B399">
         <v>1</v>
@@ -4929,7 +4948,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>389</v>
+        <v>347</v>
       </c>
       <c r="B400">
         <v>1</v>
@@ -4937,7 +4956,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>390</v>
+        <v>348</v>
       </c>
       <c r="B401">
         <v>1</v>
@@ -4945,23 +4964,23 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>391</v>
+        <v>349</v>
       </c>
       <c r="B402">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="B403">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>393</v>
+        <v>351</v>
       </c>
       <c r="B404">
         <v>1</v>
@@ -4969,7 +4988,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>394</v>
+        <v>352</v>
       </c>
       <c r="B405">
         <v>1</v>
@@ -4977,7 +4996,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>395</v>
+        <v>352</v>
       </c>
       <c r="B406">
         <v>1</v>
@@ -4985,23 +5004,23 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="B407">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>397</v>
+        <v>354</v>
       </c>
       <c r="B408">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
       <c r="B409">
         <v>1</v>
@@ -5009,7 +5028,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>399</v>
+        <v>356</v>
       </c>
       <c r="B410">
         <v>1</v>
@@ -5017,7 +5036,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="B411">
         <v>1</v>
@@ -5025,7 +5044,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="B412">
         <v>1</v>
@@ -5033,7 +5052,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>401</v>
+        <v>359</v>
       </c>
       <c r="B413">
         <v>1</v>
@@ -5041,7 +5060,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>402</v>
+        <v>360</v>
       </c>
       <c r="B414">
         <v>1</v>
@@ -5049,7 +5068,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="B415">
         <v>1</v>
@@ -5057,7 +5076,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="B416">
         <v>1</v>
@@ -5065,7 +5084,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>405</v>
+        <v>363</v>
       </c>
       <c r="B417">
         <v>1</v>
@@ -5073,7 +5092,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>406</v>
+        <v>364</v>
       </c>
       <c r="B418">
         <v>1</v>
@@ -5081,7 +5100,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>407</v>
+        <v>365</v>
       </c>
       <c r="B419">
         <v>1</v>
@@ -5089,7 +5108,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>408</v>
+        <v>366</v>
       </c>
       <c r="B420">
         <v>1</v>
@@ -5097,7 +5116,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>409</v>
+        <v>367</v>
       </c>
       <c r="B421">
         <v>1</v>
@@ -5105,7 +5124,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>410</v>
+        <v>368</v>
       </c>
       <c r="B422">
         <v>1</v>
@@ -5113,7 +5132,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>411</v>
+        <v>369</v>
       </c>
       <c r="B423">
         <v>1</v>
@@ -5121,7 +5140,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>412</v>
+        <v>370</v>
       </c>
       <c r="B424">
         <v>1</v>
@@ -5129,7 +5148,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>413</v>
+        <v>371</v>
       </c>
       <c r="B425">
         <v>1</v>
@@ -5137,7 +5156,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>414</v>
+        <v>372</v>
       </c>
       <c r="B426">
         <v>1</v>
@@ -5145,7 +5164,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="B427">
         <v>1</v>
@@ -5153,7 +5172,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>416</v>
+        <v>374</v>
       </c>
       <c r="B428">
         <v>1</v>
@@ -5161,7 +5180,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>417</v>
+        <v>375</v>
       </c>
       <c r="B429">
         <v>1</v>
@@ -5169,15 +5188,15 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>418</v>
+        <v>376</v>
       </c>
       <c r="B430">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>419</v>
+        <v>377</v>
       </c>
       <c r="B431">
         <v>1</v>
@@ -5185,7 +5204,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="B432">
         <v>1</v>
@@ -5193,15 +5212,15 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>421</v>
+        <v>379</v>
       </c>
       <c r="B433">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>422</v>
+        <v>380</v>
       </c>
       <c r="B434">
         <v>1</v>
@@ -5209,15 +5228,15 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="B435">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="B436">
         <v>1</v>
@@ -5225,7 +5244,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="B437">
         <v>1</v>
@@ -5233,15 +5252,15 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="B438">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>427</v>
+        <v>383</v>
       </c>
       <c r="B439">
         <v>1</v>
@@ -5249,7 +5268,7 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>438</v>
+        <v>384</v>
       </c>
       <c r="B440">
         <v>1</v>
@@ -5257,7 +5276,7 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>428</v>
+        <v>385</v>
       </c>
       <c r="B441">
         <v>1</v>
@@ -5265,7 +5284,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>429</v>
+        <v>386</v>
       </c>
       <c r="B442">
         <v>1</v>
@@ -5273,7 +5292,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="B443">
         <v>1</v>
@@ -5281,7 +5300,7 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>430</v>
+        <v>392</v>
       </c>
       <c r="B444">
         <v>1</v>
@@ -5289,7 +5308,7 @@
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="B445">
         <v>1</v>
@@ -5297,7 +5316,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="B446">
         <v>1</v>
@@ -5305,55 +5324,15 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>433</v>
+        <v>390</v>
       </c>
       <c r="B447">
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" t="s">
-        <v>434</v>
-      </c>
-      <c r="B448">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
-        <v>439</v>
-      </c>
-      <c r="B449">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" t="s">
-        <v>435</v>
-      </c>
-      <c r="B450">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" t="s">
-        <v>436</v>
-      </c>
-      <c r="B451">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A452" t="s">
-        <v>437</v>
-      </c>
-      <c r="B452">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B452" xr:uid="{D5E2A364-7B88-4106-9A95-3E56C3C6E261}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B110">
+  <autoFilter ref="A1:B447" xr:uid="{D5E2A364-7B88-4106-9A95-3E56C3C6E261}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B109">
     <sortCondition ref="A84"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>